<commit_message>
- Added BOM for ripples-diy
</commit_message>
<xml_diff>
--- a/ripples-diy/bom/ripples-bom.xlsx
+++ b/ripples-diy/bom/ripples-bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="0" windowWidth="22440" windowHeight="26360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="27280" yWindow="0" windowWidth="22440" windowHeight="26360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Eagle Output" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="345">
   <si>
     <t>Partlist</t>
   </si>
@@ -973,13 +973,115 @@
   </si>
   <si>
     <t>510R</t>
+  </si>
+  <si>
+    <t>621-1N5819HW-F</t>
+  </si>
+  <si>
+    <t>649-68602-110HLF</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>81-GRM188R61C104KA1D</t>
+  </si>
+  <si>
+    <t>667-EEE-FK1V470P</t>
+  </si>
+  <si>
+    <t>81-GRM185C1H470GA01J</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-100K-E3</t>
+  </si>
+  <si>
+    <t>Thonk Alpha 9mm</t>
+  </si>
+  <si>
+    <t>595-TL072CD</t>
+  </si>
+  <si>
+    <t>595-TL074CD</t>
+  </si>
+  <si>
+    <t>595-LM4040C25IDBZR</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-510-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-1.0K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-6.8K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-15K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-22K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-27K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-33K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-39K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-47K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-62K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-300K-E3</t>
+  </si>
+  <si>
+    <t>Thonk</t>
+  </si>
+  <si>
+    <t>512-MMBT3906</t>
+  </si>
+  <si>
+    <t>926-LM13700MX/NOPB</t>
+  </si>
+  <si>
+    <t>SOD323</t>
+  </si>
+  <si>
+    <t>78-1N4148WS-E3-08</t>
+  </si>
+  <si>
+    <t>77-VJ0603A561GXACBC</t>
+  </si>
+  <si>
+    <t>77-VJ0603A221GXACBC</t>
+  </si>
+  <si>
+    <t>80-C0603C224J3RACTU</t>
+  </si>
+  <si>
+    <t>667-EEE-FK1V4R7R</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>652-3296W-1-202LF</t>
+  </si>
+  <si>
+    <t>SSM2164</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1008,6 +1110,20 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1026,7 +1142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1138,8 +1254,122 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1148,8 +1378,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="225">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1205,6 +1437,63 @@
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1260,6 +1549,63 @@
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3994,10 +4340,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E36"/>
+  <dimension ref="A2:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4032,7 +4378,12 @@
       <c r="C3">
         <v>4</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="D3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="B4" t="s">
@@ -4041,7 +4392,12 @@
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="D4" t="s">
+        <v>339</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
@@ -4050,7 +4406,12 @@
       <c r="C5">
         <v>7</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="D5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" t="s">
@@ -4059,7 +4420,12 @@
       <c r="C6">
         <v>8</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="D6" t="s">
+        <v>314</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" t="s">
@@ -4068,28 +4434,39 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="D7" t="s">
+        <v>340</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>341</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="B9" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>315</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4102,6 +4479,9 @@
       <c r="C10">
         <v>2</v>
       </c>
+      <c r="D10" t="s">
+        <v>311</v>
+      </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
@@ -4111,219 +4491,331 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="D11" t="s">
+        <v>337</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>296</v>
-      </c>
-      <c r="B13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
+      <c r="B13" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="E13" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="B14" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
+      <c r="D14" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="B15" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="7">
+        <v>9</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>299</v>
+      </c>
+      <c r="B19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="B17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>297</v>
-      </c>
-      <c r="B18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>298</v>
-      </c>
-      <c r="B19" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B20" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>300</v>
-      </c>
-      <c r="B21" t="s">
-        <v>174</v>
+        <v>301</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>310</v>
       </c>
       <c r="C21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>301</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>310</v>
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>322</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" t="s">
+        <v>302</v>
       </c>
       <c r="C22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>323</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="B23" t="s">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="C23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>324</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="B24" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" t="s">
+        <v>325</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="B25" t="s">
-        <v>265</v>
+        <v>219</v>
       </c>
       <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>326</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="B26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" t="s">
+        <v>327</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="B27" t="s">
-        <v>235</v>
+        <v>181</v>
       </c>
       <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>328</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="B28" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
       <c r="C28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>329</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="B29" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" t="s">
+        <v>330</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="B30" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>331</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>202</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>317</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>332</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>308</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="B31" t="s">
-        <v>238</v>
-      </c>
-      <c r="C31">
+      <c r="D34" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="B35" t="s">
+        <v>303</v>
+      </c>
+      <c r="C35">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="B32" t="s">
-        <v>202</v>
-      </c>
-      <c r="C32">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="B33" t="s">
-        <v>216</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>308</v>
-      </c>
-      <c r="B35" t="s">
-        <v>195</v>
-      </c>
-      <c r="C35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="B36" t="s">
-        <v>303</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
+      <c r="D35" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="E21:E32 E3:E7" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Corrected Ripples BOM - LM4040 part was incorrect (2.5V instead of 5.0V)
</commit_message>
<xml_diff>
--- a/ripples-diy/bom/ripples-bom.xlsx
+++ b/ripples-diy/bom/ripples-bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27280" yWindow="0" windowWidth="22440" windowHeight="26360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8100" yWindow="0" windowWidth="22440" windowHeight="26360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Eagle Output" sheetId="1" r:id="rId1"/>
@@ -1005,9 +1005,6 @@
     <t>595-TL074CD</t>
   </si>
   <si>
-    <t>595-LM4040C25IDBZR</t>
-  </si>
-  <si>
     <t>71-CRCW0603-510-E3</t>
   </si>
   <si>
@@ -1068,13 +1065,16 @@
     <t>667-EEE-FK1V4R7R</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>652-3296W-1-202LF</t>
   </si>
   <si>
-    <t>SSM2164</t>
+    <t>522-LM4040B50FTA</t>
+  </si>
+  <si>
+    <t>Small Bear</t>
+  </si>
+  <si>
+    <t>SSM2164 (substitute Coolaudio V2164)</t>
   </si>
 </sst>
 </file>
@@ -4343,7 +4343,7 @@
   <dimension ref="A2:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4393,7 +4393,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>313</v>
@@ -4407,7 +4407,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>313</v>
@@ -4435,7 +4435,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>313</v>
@@ -4449,7 +4449,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E8" t="s">
         <v>58</v>
@@ -4492,10 +4492,10 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -4520,7 +4520,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E13" t="s">
         <v>344</v>
@@ -4534,7 +4534,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -4556,7 +4556,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>321</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -4570,7 +4570,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -4612,7 +4612,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -4626,7 +4626,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>313</v>
@@ -4640,7 +4640,7 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>313</v>
@@ -4654,7 +4654,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>313</v>
@@ -4668,7 +4668,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>313</v>
@@ -4682,7 +4682,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>313</v>
@@ -4696,7 +4696,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>313</v>
@@ -4710,7 +4710,7 @@
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>313</v>
@@ -4724,7 +4724,7 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>313</v>
@@ -4738,7 +4738,7 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>313</v>
@@ -4752,7 +4752,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>313</v>
@@ -4780,7 +4780,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>313</v>
@@ -4808,7 +4808,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>